<commit_message>
Changes to the Services and Code Generator
</commit_message>
<xml_diff>
--- a/CodeGeneratorFlutterModel.xlsx
+++ b/CodeGeneratorFlutterModel.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashrafkabir/Documents/projects/planb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashrafkabir/Desktop/projects/planb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ED678F5-0201-7C44-A750-93866C687869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6945FE6D-D2BC-2844-BFD3-5A7F1EF677AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13760" xr2:uid="{522547A4-0E54-C049-8414-39FDB5688C0E}"/>
+    <workbookView xWindow="480" yWindow="760" windowWidth="25040" windowHeight="13760" xr2:uid="{522547A4-0E54-C049-8414-39FDB5688C0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>{</t>
   </si>
@@ -74,37 +75,52 @@
     <t>profile information</t>
   </si>
   <si>
-    <t>User_Address</t>
-  </si>
-  <si>
-    <t>User_Category</t>
-  </si>
-  <si>
-    <t>User_Designation</t>
-  </si>
-  <si>
-    <t>User_Email</t>
-  </si>
-  <si>
-    <t>User_Interaction</t>
-  </si>
-  <si>
-    <t>User_Likability</t>
-  </si>
-  <si>
-    <t>User_Name</t>
-  </si>
-  <si>
-    <t>User_Phone</t>
-  </si>
-  <si>
-    <t>User_Phone2</t>
-  </si>
-  <si>
-    <t>User_Pic</t>
-  </si>
-  <si>
-    <t>User_Profile</t>
+    <t>Post_Id</t>
+  </si>
+  <si>
+    <t>Class_Id</t>
+  </si>
+  <si>
+    <t>Post_Audience</t>
+  </si>
+  <si>
+    <t>Post_Category</t>
+  </si>
+  <si>
+    <t>Post_Type</t>
+  </si>
+  <si>
+    <t>Post_Time</t>
+  </si>
+  <si>
+    <t>Post_Title</t>
+  </si>
+  <si>
+    <t>Post_Pic</t>
+  </si>
+  <si>
+    <t>Post_Author</t>
+  </si>
+  <si>
+    <t>Post_Body</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Emotions</t>
+  </si>
+  <si>
+    <t>Poll_Id</t>
+  </si>
+  <si>
+    <t>Homework_Id</t>
+  </si>
+  <si>
+    <t>Event_Id</t>
+  </si>
+  <si>
+    <t>Action_Id</t>
   </si>
 </sst>
 </file>
@@ -456,24 +472,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A852B87-2424-E443-AC3A-7D10941348E6}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E12"/>
+      <selection activeCell="F2" sqref="F2:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="49.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>13</v>
       </c>
@@ -481,15 +499,27 @@
         <v>2</v>
       </c>
       <c r="D2" t="str">
+        <f>"final String "&amp;B2&amp;";"</f>
+        <v>final String Post_Id;</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"this."&amp;B2&amp;","</f>
+        <v>this.Post_Id,</v>
+      </c>
+      <c r="F2" t="str">
+        <f>B2&amp;": "&amp;"json['"&amp;B2&amp;"'],"</f>
+        <v>Post_Id: json['Post_Id'],</v>
+      </c>
+      <c r="G2" t="str">
         <f>"const " &amp; B2 &amp; "  = requestBody." &amp; B2 &amp; ";"</f>
-        <v>const User_Address  = requestBody.User_Address;</v>
-      </c>
-      <c r="E2" t="str">
+        <v>const Post_Id  = requestBody.Post_Id;</v>
+      </c>
+      <c r="H2" t="str">
         <f>B2 &amp; ":" &amp; B2 &amp; ","</f>
-        <v>User_Address:User_Address,</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>Post_Id:Post_Id,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -497,15 +527,27 @@
         <v>3</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D12" si="0">"const " &amp; B3 &amp; "  = requestBody." &amp; B3 &amp; ";"</f>
-        <v>const User_Category  = requestBody.User_Category;</v>
+        <f t="shared" ref="D3:D17" si="0">"final String "&amp;B3&amp;";"</f>
+        <v>final String Class_Id;</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E12" si="1">B3 &amp; ":" &amp; B3 &amp; ","</f>
-        <v>User_Category:User_Category,</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <f t="shared" ref="E3:E17" si="1">"this."&amp;B3&amp;","</f>
+        <v>this.Class_Id,</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F17" si="2">B3&amp;": "&amp;"json['"&amp;B3&amp;"'],"</f>
+        <v>Class_Id: json['Class_Id'],</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G12" si="3">"const " &amp; B3 &amp; "  = requestBody." &amp; B3 &amp; ";"</f>
+        <v>const Class_Id  = requestBody.Class_Id;</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H12" si="4">B3 &amp; ":" &amp; B3 &amp; ","</f>
+        <v>Class_Id:Class_Id,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -514,14 +556,26 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>const User_Designation  = requestBody.User_Designation;</v>
+        <v>final String Post_Audience;</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>User_Designation:User_Designation,</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>this.Post_Audience,</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>Post_Audience: json['Post_Audience'],</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="3"/>
+        <v>const Post_Audience  = requestBody.Post_Audience;</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="4"/>
+        <v>Post_Audience:Post_Audience,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -530,14 +584,26 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>const User_Email  = requestBody.User_Email;</v>
+        <v>final String Post_Category;</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>User_Email:User_Email,</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>this.Post_Category,</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>Post_Category: json['Post_Category'],</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="3"/>
+        <v>const Post_Category  = requestBody.Post_Category;</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="4"/>
+        <v>Post_Category:Post_Category,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -546,14 +612,26 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>const User_Interaction  = requestBody.User_Interaction;</v>
+        <v>final String Post_Type;</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>User_Interaction:User_Interaction,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>this.Post_Type,</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>Post_Type: json['Post_Type'],</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="3"/>
+        <v>const Post_Type  = requestBody.Post_Type;</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="4"/>
+        <v>Post_Type:Post_Type,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -562,14 +640,26 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>const User_Likability  = requestBody.User_Likability;</v>
+        <v>final String Post_Time;</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>User_Likability:User_Likability,</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>this.Post_Time,</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>Post_Time: json['Post_Time'],</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="3"/>
+        <v>const Post_Time  = requestBody.Post_Time;</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="4"/>
+        <v>Post_Time:Post_Time,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -578,14 +668,26 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>const User_Name  = requestBody.User_Name;</v>
+        <v>final String Post_Title;</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>User_Name:User_Name,</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>this.Post_Title,</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>Post_Title: json['Post_Title'],</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="3"/>
+        <v>const Post_Title  = requestBody.Post_Title;</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="4"/>
+        <v>Post_Title:Post_Title,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -594,14 +696,26 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>const User_Phone  = requestBody.User_Phone;</v>
+        <v>final String Post_Pic;</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>User_Phone:User_Phone,</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>this.Post_Pic,</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>Post_Pic: json['Post_Pic'],</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="3"/>
+        <v>const Post_Pic  = requestBody.Post_Pic;</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="4"/>
+        <v>Post_Pic:Post_Pic,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -610,14 +724,26 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>const User_Phone2  = requestBody.User_Phone2;</v>
+        <v>final String Post_Author;</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>User_Phone2:User_Phone2,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>this.Post_Author,</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>Post_Author: json['Post_Author'],</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="3"/>
+        <v>const Post_Author  = requestBody.Post_Author;</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="4"/>
+        <v>Post_Author:Post_Author,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -626,14 +752,26 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>const User_Pic  = requestBody.User_Pic;</v>
+        <v>final String Post_Body;</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>User_Pic:User_Pic,</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>this.Post_Body,</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>Post_Body: json['Post_Body'],</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="3"/>
+        <v>const Post_Body  = requestBody.Post_Body;</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="4"/>
+        <v>Post_Body:Post_Body,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -642,16 +780,166 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>const User_Profile  = requestBody.User_Profile;</v>
+        <v>final String Comments;</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>User_Profile:User_Profile,</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>this.Comments,</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="2"/>
+        <v>Comments: json['Comments'],</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="3"/>
+        <v>const Comments  = requestBody.Comments;</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="4"/>
+        <v>Comments:Comments,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>final String Emotions;</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>this.Emotions,</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="2"/>
+        <v>Emotions: json['Emotions'],</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ref="G13:G17" si="5">"const " &amp; B13 &amp; "  = requestBody." &amp; B13 &amp; ";"</f>
+        <v>const Emotions  = requestBody.Emotions;</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" ref="H13:H17" si="6">B13 &amp; ":" &amp; B13 &amp; ","</f>
+        <v>Emotions:Emotions,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>final String Poll_Id;</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>this.Poll_Id,</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="2"/>
+        <v>Poll_Id: json['Poll_Id'],</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="5"/>
+        <v>const Poll_Id  = requestBody.Poll_Id;</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="6"/>
+        <v>Poll_Id:Poll_Id,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>final String Homework_Id;</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>this.Homework_Id,</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="2"/>
+        <v>Homework_Id: json['Homework_Id'],</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="5"/>
+        <v>const Homework_Id  = requestBody.Homework_Id;</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="6"/>
+        <v>Homework_Id:Homework_Id,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>final String Event_Id;</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>this.Event_Id,</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v>Event_Id: json['Event_Id'],</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="5"/>
+        <v>const Event_Id  = requestBody.Event_Id;</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="6"/>
+        <v>Event_Id:Event_Id,</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>final String Action_Id;</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>this.Action_Id,</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="2"/>
+        <v>Action_Id: json['Action_Id'],</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="5"/>
+        <v>const Action_Id  = requestBody.Action_Id;</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="6"/>
+        <v>Action_Id:Action_Id,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>